<commit_message>
aggiornamento indicatori Retail e rename xls
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
+++ b/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="410">
   <si>
     <t>Verificare/Cambiare tutte le formule indeterminate</t>
   </si>
@@ -3464,8 +3464,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AE129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7771,8 +7771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9240,10 +9240,10 @@
   <dimension ref="B1:AH45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="P11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -9317,11 +9317,11 @@
       </c>
       <c r="Q1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="R1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="S1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -10851,7 +10851,7 @@
       </c>
       <c r="AB1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="AC1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="AD1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="AE1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -13731,10 +13731,10 @@
   <dimension ref="B1:FU16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3:T3"/>
+      <selection pane="bottomRight" activeCell="AP14" sqref="AP14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -13810,7 +13810,7 @@
       </c>
       <c r="Q1" s="65" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="R1" s="65" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -13818,7 +13818,7 @@
       </c>
       <c r="S1" s="65" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="T1" s="65" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -15050,7 +15050,9 @@
       <c r="DT3" s="69"/>
       <c r="DU3" s="69"/>
       <c r="DV3" s="69"/>
-      <c r="DW3" s="69"/>
+      <c r="DW3" s="85" t="s">
+        <v>259</v>
+      </c>
       <c r="DX3" s="71" t="s">
         <v>267</v>
       </c>
@@ -15311,9 +15313,15 @@
       <c r="EG4" s="71" t="s">
         <v>267</v>
       </c>
-      <c r="EH4" s="69"/>
-      <c r="EI4" s="69"/>
-      <c r="EJ4" s="69"/>
+      <c r="EH4" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="EI4" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="EJ4" s="85" t="s">
+        <v>259</v>
+      </c>
       <c r="EK4" s="69"/>
       <c r="EL4" s="69"/>
       <c r="EM4" s="69"/>
@@ -16479,7 +16487,7 @@
       </c>
       <c r="DW8" s="62">
         <f t="shared" si="81"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="DX8" s="62"/>
       <c r="DY8" s="62"/>
@@ -16493,15 +16501,15 @@
       <c r="EG8" s="62"/>
       <c r="EH8" s="62">
         <f t="shared" ref="EH8:FT8" si="82">COUNTBLANK(EH3:EH7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="EI8" s="62">
         <f t="shared" si="82"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="EJ8" s="62">
         <f t="shared" si="82"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="EK8" s="62">
         <f t="shared" si="82"/>

</xml_diff>

<commit_message>
test ispro e isba
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
+++ b/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9216" windowHeight="5340" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9216" windowHeight="5340" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Elenco_attività" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Plan team" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elenco_attività!$B$1:$J$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elenco_attività!$B$1:$J$151</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="467">
   <si>
     <t>Verificare/Cambiare tutte le formule indeterminate</t>
   </si>
@@ -1422,6 +1422,18 @@
   </si>
   <si>
     <t>APP2.0 - Migrazione</t>
+  </si>
+  <si>
+    <t>Override - incrocio assegni (BR34)</t>
+  </si>
+  <si>
+    <t>18/04 dati in sviluppo, 24/04 in syt. 27/04 inizio UAT</t>
+  </si>
+  <si>
+    <t>UAT 24/04</t>
+  </si>
+  <si>
+    <t>dati 18/04</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2195,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="147">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3910,10 +3982,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AE150"/>
+  <dimension ref="A1:AE151"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="D102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6802,7 +6874,7 @@
     </row>
     <row r="101" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B101" s="7">
-        <f t="shared" ref="B101:B130" si="4">+B100+1</f>
+        <f t="shared" ref="B101:B131" si="4">+B100+1</f>
         <v>100</v>
       </c>
       <c r="C101" s="10" t="s">
@@ -7552,75 +7624,82 @@
       </c>
       <c r="J130" s="1"/>
     </row>
-    <row r="131" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C131" s="31"/>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B131" s="7">
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="D131" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="5">
+        <v>3</v>
+      </c>
+      <c r="I131" s="5">
+        <v>2</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="132" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="91" t="s">
+      <c r="C132" s="31"/>
+    </row>
+    <row r="133" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B133" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="C132" s="92" t="s">
+      <c r="C133" s="92" t="s">
         <v>417</v>
       </c>
-      <c r="D132" s="91" t="s">
+      <c r="D133" s="91" t="s">
         <v>418</v>
       </c>
-      <c r="E132" s="90" t="s">
+      <c r="E133" s="90" t="s">
         <v>415</v>
       </c>
-      <c r="F132" s="90" t="s">
+      <c r="F133" s="90" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="133" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="94" t="s">
+    <row r="134" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="94" t="s">
         <v>146</v>
       </c>
-      <c r="C133" s="95" t="s">
+      <c r="C134" s="95" t="s">
         <v>420</v>
       </c>
-      <c r="D133" s="96">
+      <c r="D134" s="96">
         <v>42815</v>
       </c>
-      <c r="E133" s="93" t="s">
+      <c r="E134" s="93" t="s">
         <v>419</v>
       </c>
-      <c r="F133" s="93">
+      <c r="F134" s="93">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="98" t="s">
+    <row r="135" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="98" t="s">
         <v>422</v>
       </c>
-      <c r="C134" s="99" t="s">
+      <c r="C135" s="99" t="s">
         <v>423</v>
       </c>
-      <c r="D134" s="100">
+      <c r="D135" s="100">
         <v>42814</v>
       </c>
-      <c r="E134" s="97" t="s">
+      <c r="E135" s="97" t="s">
         <v>421</v>
       </c>
-      <c r="F134" s="97">
+      <c r="F135" s="97">
         <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B135" s="102" t="s">
-        <v>425</v>
-      </c>
-      <c r="C135" s="103" t="s">
-        <v>426</v>
-      </c>
-      <c r="D135" s="104">
-        <v>42814</v>
-      </c>
-      <c r="E135" s="101" t="s">
-        <v>424</v>
-      </c>
-      <c r="F135" s="101">
-        <v>1</v>
       </c>
     </row>
     <row r="136" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7628,13 +7707,13 @@
         <v>425</v>
       </c>
       <c r="C136" s="103" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D136" s="104">
-        <v>42816</v>
+        <v>42814</v>
       </c>
       <c r="E136" s="101" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F136" s="101">
         <v>1</v>
@@ -7645,10 +7724,10 @@
         <v>425</v>
       </c>
       <c r="C137" s="103" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D137" s="104">
-        <v>42818</v>
+        <v>42816</v>
       </c>
       <c r="E137" s="101" t="s">
         <v>427</v>
@@ -7662,13 +7741,13 @@
         <v>425</v>
       </c>
       <c r="C138" s="103" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D138" s="104">
         <v>42818</v>
       </c>
       <c r="E138" s="101" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="F138" s="101">
         <v>1</v>
@@ -7679,16 +7758,16 @@
         <v>425</v>
       </c>
       <c r="C139" s="103" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D139" s="104">
         <v>42818</v>
       </c>
       <c r="E139" s="101" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F139" s="101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -7696,13 +7775,13 @@
         <v>425</v>
       </c>
       <c r="C140" s="103" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D140" s="104">
         <v>42818</v>
       </c>
       <c r="E140" s="101" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F140" s="101">
         <v>0</v>
@@ -7713,13 +7792,13 @@
         <v>425</v>
       </c>
       <c r="C141" s="103" t="s">
-        <v>433</v>
-      </c>
-      <c r="D141" s="102" t="s">
-        <v>434</v>
+        <v>432</v>
+      </c>
+      <c r="D141" s="104">
+        <v>42818</v>
       </c>
       <c r="E141" s="101" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="F141" s="101">
         <v>0</v>
@@ -7730,13 +7809,13 @@
         <v>425</v>
       </c>
       <c r="C142" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D142" s="102" t="s">
         <v>434</v>
       </c>
       <c r="E142" s="101" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="F142" s="101">
         <v>0</v>
@@ -7747,13 +7826,13 @@
         <v>425</v>
       </c>
       <c r="C143" s="103" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D143" s="102" t="s">
         <v>434</v>
       </c>
       <c r="E143" s="101" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="F143" s="101">
         <v>0</v>
@@ -7764,83 +7843,83 @@
         <v>425</v>
       </c>
       <c r="C144" s="103" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D144" s="102" t="s">
         <v>434</v>
       </c>
       <c r="E144" s="101" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F144" s="101">
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="106" t="s">
-        <v>439</v>
-      </c>
-      <c r="C145" s="107" t="s">
-        <v>440</v>
-      </c>
-      <c r="D145" s="108">
-        <v>42815</v>
-      </c>
-      <c r="E145" s="105" t="s">
-        <v>436</v>
-      </c>
-      <c r="F145" s="105">
-        <v>1</v>
+      <c r="B145" s="102" t="s">
+        <v>425</v>
+      </c>
+      <c r="C145" s="103" t="s">
+        <v>438</v>
+      </c>
+      <c r="D145" s="102" t="s">
+        <v>434</v>
+      </c>
+      <c r="E145" s="101" t="s">
+        <v>427</v>
+      </c>
+      <c r="F145" s="101">
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="106" t="s">
+        <v>439</v>
+      </c>
+      <c r="C146" s="107" t="s">
+        <v>440</v>
+      </c>
+      <c r="D146" s="108">
+        <v>42815</v>
+      </c>
+      <c r="E146" s="105" t="s">
+        <v>436</v>
+      </c>
+      <c r="F146" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="106" t="s">
         <v>139</v>
       </c>
-      <c r="C146" s="107" t="s">
+      <c r="C147" s="107" t="s">
         <v>441</v>
       </c>
-      <c r="D146" s="108">
+      <c r="D147" s="108">
         <v>42817</v>
       </c>
-      <c r="E146" s="105" t="s">
+      <c r="E147" s="105" t="s">
         <v>427</v>
       </c>
-      <c r="F146" s="105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="110" t="s">
+      <c r="F147" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="C147" s="111" t="s">
+      <c r="C148" s="111" t="s">
         <v>442</v>
       </c>
-      <c r="D147" s="112">
+      <c r="D148" s="112">
         <v>42824</v>
       </c>
-      <c r="E147" s="109" t="s">
+      <c r="E148" s="109" t="s">
         <v>419</v>
       </c>
-      <c r="F147" s="109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="114" t="s">
-        <v>443</v>
-      </c>
-      <c r="C148" s="115" t="s">
-        <v>444</v>
-      </c>
-      <c r="D148" s="116">
-        <v>42822</v>
-      </c>
-      <c r="E148" s="113" t="s">
-        <v>436</v>
-      </c>
-      <c r="F148" s="113">
+      <c r="F148" s="109">
         <v>0</v>
       </c>
     </row>
@@ -7849,13 +7928,13 @@
         <v>443</v>
       </c>
       <c r="C149" s="115" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D149" s="116">
-        <v>42825</v>
+        <v>42822</v>
       </c>
       <c r="E149" s="113" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="F149" s="113">
         <v>0</v>
@@ -7866,7 +7945,7 @@
         <v>443</v>
       </c>
       <c r="C150" s="115" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D150" s="116">
         <v>42825</v>
@@ -7878,714 +7957,746 @@
         <v>0</v>
       </c>
     </row>
+    <row r="151" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="C151" s="115" t="s">
+        <v>446</v>
+      </c>
+      <c r="D151" s="116">
+        <v>42825</v>
+      </c>
+      <c r="E151" s="113" t="s">
+        <v>419</v>
+      </c>
+      <c r="F151" s="113">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:J150">
+  <autoFilter ref="B1:J151">
     <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E1:G16 F2:G70 E18:G68 E113:G113">
+    <cfRule type="cellIs" dxfId="146" priority="185" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:G17 G18:G44">
+    <cfRule type="cellIs" dxfId="145" priority="184" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69:G69">
+    <cfRule type="cellIs" dxfId="144" priority="183" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:G70">
+    <cfRule type="cellIs" dxfId="143" priority="182" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F71:G71">
+    <cfRule type="cellIs" dxfId="142" priority="181" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71:G71">
+    <cfRule type="cellIs" dxfId="141" priority="180" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F72:G72">
     <cfRule type="cellIs" dxfId="140" priority="179" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:G17 G18:G44">
+  <conditionalFormatting sqref="E72:G72">
     <cfRule type="cellIs" dxfId="139" priority="178" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69:G69">
+  <conditionalFormatting sqref="F73:G73">
     <cfRule type="cellIs" dxfId="138" priority="177" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70:G70">
+  <conditionalFormatting sqref="E73:G73">
     <cfRule type="cellIs" dxfId="137" priority="176" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F71:G71">
+  <conditionalFormatting sqref="F74:G74">
     <cfRule type="cellIs" dxfId="136" priority="175" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E71:G71">
+  <conditionalFormatting sqref="E74:G74">
     <cfRule type="cellIs" dxfId="135" priority="174" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F72:G72">
+  <conditionalFormatting sqref="F75:G75">
     <cfRule type="cellIs" dxfId="134" priority="173" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72:G72">
+  <conditionalFormatting sqref="E75:G75">
     <cfRule type="cellIs" dxfId="133" priority="172" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:G73">
+  <conditionalFormatting sqref="F76:G76">
     <cfRule type="cellIs" dxfId="132" priority="171" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73:G73">
+  <conditionalFormatting sqref="E76:G76">
     <cfRule type="cellIs" dxfId="131" priority="170" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F74:G74">
+  <conditionalFormatting sqref="E69">
     <cfRule type="cellIs" dxfId="130" priority="169" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:G74">
+  <conditionalFormatting sqref="F77:G77">
     <cfRule type="cellIs" dxfId="129" priority="168" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F75:G75">
+  <conditionalFormatting sqref="E77:G77">
     <cfRule type="cellIs" dxfId="128" priority="167" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75:G75">
+  <conditionalFormatting sqref="F78:G78">
     <cfRule type="cellIs" dxfId="127" priority="166" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F76:G76">
+  <conditionalFormatting sqref="E78:G78">
     <cfRule type="cellIs" dxfId="126" priority="165" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76:G76">
+  <conditionalFormatting sqref="G46">
     <cfRule type="cellIs" dxfId="125" priority="164" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="124" priority="163" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F77:G77">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="123" priority="162" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:G77">
+  <conditionalFormatting sqref="G51:G52">
     <cfRule type="cellIs" dxfId="122" priority="161" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F78:G78">
+  <conditionalFormatting sqref="G45">
     <cfRule type="cellIs" dxfId="121" priority="160" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:G78">
+  <conditionalFormatting sqref="F79:G80">
     <cfRule type="cellIs" dxfId="120" priority="159" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="E79:G79 F80:G80">
     <cfRule type="cellIs" dxfId="119" priority="158" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
+  <conditionalFormatting sqref="E80">
     <cfRule type="cellIs" dxfId="118" priority="157" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="117" priority="156" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51:G52">
-    <cfRule type="cellIs" dxfId="116" priority="155" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="cellIs" dxfId="115" priority="154" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F79:G80">
-    <cfRule type="cellIs" dxfId="114" priority="153" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:G79 F80:G80">
-    <cfRule type="cellIs" dxfId="113" priority="152" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E80">
-    <cfRule type="cellIs" dxfId="112" priority="151" operator="lessThan">
+  <conditionalFormatting sqref="F81:G82">
+    <cfRule type="cellIs" dxfId="117" priority="153" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:G82">
-    <cfRule type="cellIs" dxfId="111" priority="147" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81:G82">
-    <cfRule type="cellIs" dxfId="110" priority="146" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="152" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81:E82">
-    <cfRule type="cellIs" dxfId="109" priority="145" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="151" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83:G83">
-    <cfRule type="cellIs" dxfId="108" priority="144" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="150" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83:G83">
-    <cfRule type="cellIs" dxfId="107" priority="143" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="149" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F84:G84">
+    <cfRule type="cellIs" dxfId="112" priority="147" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84:G84">
+    <cfRule type="cellIs" dxfId="111" priority="146" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84">
+    <cfRule type="cellIs" dxfId="110" priority="145" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F86:G86">
+    <cfRule type="cellIs" dxfId="109" priority="144" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F86:G86">
+    <cfRule type="cellIs" dxfId="108" priority="143" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86">
+    <cfRule type="cellIs" dxfId="107" priority="142" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F87:G87">
     <cfRule type="cellIs" dxfId="106" priority="141" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84:G84">
+  <conditionalFormatting sqref="F87:G87">
     <cfRule type="cellIs" dxfId="105" priority="140" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E87">
     <cfRule type="cellIs" dxfId="104" priority="139" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:G86">
+  <conditionalFormatting sqref="F85:G85">
     <cfRule type="cellIs" dxfId="103" priority="138" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:G86">
+  <conditionalFormatting sqref="F85:G85">
     <cfRule type="cellIs" dxfId="102" priority="137" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E86">
+  <conditionalFormatting sqref="E85">
     <cfRule type="cellIs" dxfId="101" priority="136" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:G87">
+  <conditionalFormatting sqref="F88:G88">
     <cfRule type="cellIs" dxfId="100" priority="135" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:G87">
+  <conditionalFormatting sqref="F88:G88">
     <cfRule type="cellIs" dxfId="99" priority="134" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E88">
     <cfRule type="cellIs" dxfId="98" priority="133" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85:G85">
+  <conditionalFormatting sqref="F90:G90">
     <cfRule type="cellIs" dxfId="97" priority="132" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85:G85">
+  <conditionalFormatting sqref="F90:G90">
     <cfRule type="cellIs" dxfId="96" priority="131" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E90">
     <cfRule type="cellIs" dxfId="95" priority="130" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:G88">
+  <conditionalFormatting sqref="F91:G91">
     <cfRule type="cellIs" dxfId="94" priority="129" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:G88">
+  <conditionalFormatting sqref="F91:G91">
     <cfRule type="cellIs" dxfId="93" priority="128" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88">
+  <conditionalFormatting sqref="E91">
     <cfRule type="cellIs" dxfId="92" priority="127" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90:G90">
+  <conditionalFormatting sqref="F89">
     <cfRule type="cellIs" dxfId="91" priority="126" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90:G90">
+  <conditionalFormatting sqref="F89">
     <cfRule type="cellIs" dxfId="90" priority="125" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
+  <conditionalFormatting sqref="E89">
     <cfRule type="cellIs" dxfId="89" priority="124" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:G91">
-    <cfRule type="cellIs" dxfId="88" priority="123" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F91:G91">
-    <cfRule type="cellIs" dxfId="87" priority="122" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="86" priority="121" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F89">
-    <cfRule type="cellIs" dxfId="85" priority="120" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F89">
-    <cfRule type="cellIs" dxfId="84" priority="119" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E89">
-    <cfRule type="cellIs" dxfId="83" priority="118" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="82" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="121" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="81" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="113" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F95:G95">
-    <cfRule type="cellIs" dxfId="80" priority="104" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="110" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95:G95">
-    <cfRule type="cellIs" dxfId="79" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="109" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94">
+    <cfRule type="cellIs" dxfId="84" priority="106" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E96">
+    <cfRule type="cellIs" dxfId="83" priority="105" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97">
+    <cfRule type="cellIs" dxfId="82" priority="104" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97">
+    <cfRule type="cellIs" dxfId="81" priority="103" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97">
+    <cfRule type="cellIs" dxfId="80" priority="102" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F98">
+    <cfRule type="cellIs" dxfId="79" priority="101" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F98">
     <cfRule type="cellIs" dxfId="78" priority="100" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="E98">
     <cfRule type="cellIs" dxfId="77" priority="99" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
-    <cfRule type="cellIs" dxfId="76" priority="98" operator="lessThan">
+  <conditionalFormatting sqref="E99:E100">
+    <cfRule type="cellIs" dxfId="76" priority="93" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
-    <cfRule type="cellIs" dxfId="75" priority="97" operator="lessThan">
+  <conditionalFormatting sqref="F101:G101 F99:F100">
+    <cfRule type="cellIs" dxfId="75" priority="95" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="74" priority="96" operator="lessThan">
+  <conditionalFormatting sqref="F101:G101 F99:F100">
+    <cfRule type="cellIs" dxfId="74" priority="94" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
-    <cfRule type="cellIs" dxfId="73" priority="95" operator="lessThan">
+  <conditionalFormatting sqref="E102">
+    <cfRule type="cellIs" dxfId="73" priority="90" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
-    <cfRule type="cellIs" dxfId="72" priority="94" operator="lessThan">
+  <conditionalFormatting sqref="F102:G102">
+    <cfRule type="cellIs" dxfId="72" priority="92" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E98">
-    <cfRule type="cellIs" dxfId="71" priority="93" operator="lessThan">
+  <conditionalFormatting sqref="F102:G102">
+    <cfRule type="cellIs" dxfId="71" priority="91" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E99:E100">
+  <conditionalFormatting sqref="E103">
     <cfRule type="cellIs" dxfId="70" priority="87" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101:G101 F99:F100">
+  <conditionalFormatting sqref="F103:G103">
     <cfRule type="cellIs" dxfId="69" priority="89" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101:G101 F99:F100">
+  <conditionalFormatting sqref="F103:G103">
     <cfRule type="cellIs" dxfId="68" priority="88" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E102">
+  <conditionalFormatting sqref="E104">
     <cfRule type="cellIs" dxfId="67" priority="84" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102:G102">
+  <conditionalFormatting sqref="F104:G104">
     <cfRule type="cellIs" dxfId="66" priority="86" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102:G102">
+  <conditionalFormatting sqref="F104:G104">
     <cfRule type="cellIs" dxfId="65" priority="85" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E103">
-    <cfRule type="cellIs" dxfId="64" priority="81" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F103:G103">
-    <cfRule type="cellIs" dxfId="63" priority="83" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F103:G103">
-    <cfRule type="cellIs" dxfId="62" priority="82" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E104">
-    <cfRule type="cellIs" dxfId="61" priority="78" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F104:G104">
-    <cfRule type="cellIs" dxfId="60" priority="80" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F104:G104">
-    <cfRule type="cellIs" dxfId="59" priority="79" operator="lessThan">
+  <conditionalFormatting sqref="G99">
+    <cfRule type="cellIs" dxfId="64" priority="83" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G99">
+    <cfRule type="cellIs" dxfId="63" priority="82" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G98">
+    <cfRule type="cellIs" dxfId="62" priority="81" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G98">
+    <cfRule type="cellIs" dxfId="61" priority="80" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G97">
+    <cfRule type="cellIs" dxfId="60" priority="79" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G97">
+    <cfRule type="cellIs" dxfId="59" priority="78" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F105:G105">
     <cfRule type="cellIs" dxfId="58" priority="77" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G99">
+  <conditionalFormatting sqref="F105:G105">
     <cfRule type="cellIs" dxfId="57" priority="76" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="E105">
     <cfRule type="cellIs" dxfId="56" priority="75" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="G100">
     <cfRule type="cellIs" dxfId="55" priority="74" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="G100">
     <cfRule type="cellIs" dxfId="54" priority="73" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="F106:G106">
     <cfRule type="cellIs" dxfId="53" priority="72" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F105:G105">
+  <conditionalFormatting sqref="F106:G106">
     <cfRule type="cellIs" dxfId="52" priority="71" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F105:G105">
+  <conditionalFormatting sqref="E106">
     <cfRule type="cellIs" dxfId="51" priority="70" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
+  <conditionalFormatting sqref="F107:G107">
     <cfRule type="cellIs" dxfId="50" priority="69" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G100">
+  <conditionalFormatting sqref="F107:G107">
     <cfRule type="cellIs" dxfId="49" priority="68" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G100">
+  <conditionalFormatting sqref="E107">
     <cfRule type="cellIs" dxfId="48" priority="67" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F106:G106">
+  <conditionalFormatting sqref="F108:G108">
     <cfRule type="cellIs" dxfId="47" priority="66" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F106:G106">
+  <conditionalFormatting sqref="F108:G108">
     <cfRule type="cellIs" dxfId="46" priority="65" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
+  <conditionalFormatting sqref="E108">
     <cfRule type="cellIs" dxfId="45" priority="64" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:G107">
+  <conditionalFormatting sqref="F109:G109">
     <cfRule type="cellIs" dxfId="44" priority="63" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:G107">
+  <conditionalFormatting sqref="F109:G109">
     <cfRule type="cellIs" dxfId="43" priority="62" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
+  <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="42" priority="61" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:G108">
-    <cfRule type="cellIs" dxfId="41" priority="60" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F108:G108">
-    <cfRule type="cellIs" dxfId="40" priority="59" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="39" priority="58" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F109:G109">
-    <cfRule type="cellIs" dxfId="38" priority="57" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F109:G109">
-    <cfRule type="cellIs" dxfId="37" priority="56" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E109">
-    <cfRule type="cellIs" dxfId="36" priority="55" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E110">
-    <cfRule type="cellIs" dxfId="35" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="58" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112">
-    <cfRule type="cellIs" dxfId="34" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="52" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F114:G117">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E111">
-    <cfRule type="cellIs" dxfId="32" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="55" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E114:E117">
-    <cfRule type="cellIs" dxfId="31" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="49" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F114:G117">
-    <cfRule type="cellIs" dxfId="30" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="50" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="cellIs" dxfId="29" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="45" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="44" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F118:G118">
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="43" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F118:G118">
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="41" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F119:G119">
+    <cfRule type="cellIs" dxfId="30" priority="37" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F119:G119">
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E119">
+    <cfRule type="cellIs" dxfId="28" priority="35" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E101">
+    <cfRule type="cellIs" dxfId="27" priority="34" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83">
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F120:G121">
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F120:G121">
     <cfRule type="cellIs" dxfId="24" priority="31" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F119:G119">
+  <conditionalFormatting sqref="E120:E121">
     <cfRule type="cellIs" dxfId="23" priority="30" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E119">
+  <conditionalFormatting sqref="F122:G122 F125:G125">
     <cfRule type="cellIs" dxfId="22" priority="29" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
+  <conditionalFormatting sqref="F122:G122 F125:G125">
     <cfRule type="cellIs" dxfId="21" priority="28" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E83">
+  <conditionalFormatting sqref="E122 E125">
     <cfRule type="cellIs" dxfId="20" priority="27" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F120:G121">
+  <conditionalFormatting sqref="F111:G112">
     <cfRule type="cellIs" dxfId="19" priority="26" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F120:G121">
+  <conditionalFormatting sqref="F110">
     <cfRule type="cellIs" dxfId="18" priority="25" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E120:E121">
+  <conditionalFormatting sqref="G110">
     <cfRule type="cellIs" dxfId="17" priority="24" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F122:G122 F125:G125">
+  <conditionalFormatting sqref="F96:G96 F93:G94">
     <cfRule type="cellIs" dxfId="16" priority="23" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F122:G122 F125:G125">
+  <conditionalFormatting sqref="F92:G92">
     <cfRule type="cellIs" dxfId="15" priority="22" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122 E125">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="lessThan">
+  <conditionalFormatting sqref="F127:G129">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F111:G112">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="lessThan">
+  <conditionalFormatting sqref="F127:G129">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F110">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="lessThan">
+  <conditionalFormatting sqref="E127:E129">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G110">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="lessThan">
+  <conditionalFormatting sqref="F126:G126">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96:G96 F93:G94">
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="lessThan">
+  <conditionalFormatting sqref="F126:G126">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F92:G92">
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="E126">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F127:G130">
+  <conditionalFormatting sqref="F123:G124">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F127:G130">
+  <conditionalFormatting sqref="F123:G124">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127:E130">
+  <conditionalFormatting sqref="E123:E124">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F126:G126">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+  <conditionalFormatting sqref="F130:G131">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F126:G126">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="F130:G131">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E126">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F123:G124">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F123:G124">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E123:E124">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="E130:E131">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10286,13 +10397,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AV54"/>
+  <dimension ref="B1:AV55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -10311,7 +10422,8 @@
     <col min="20" max="21" width="6" style="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.5" style="16" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.09765625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5" style="16" bestFit="1" customWidth="1"/>
     <col min="26" max="30" width="6.19921875" style="16" bestFit="1" customWidth="1"/>
     <col min="31" max="39" width="5.296875" style="16" bestFit="1" customWidth="1"/>
     <col min="40" max="43" width="5.69921875" style="16" bestFit="1" customWidth="1"/>
@@ -10390,11 +10502,11 @@
       </c>
       <c r="U1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="V1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="W1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -10693,7 +10805,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="23" t="str">
-        <f>VLOOKUP(B3,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B3,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>indicatori esperenziali</v>
       </c>
       <c r="D3" s="23"/>
@@ -10747,7 +10859,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="23" t="str">
-        <f>VLOOKUP(B4,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B4,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v xml:space="preserve">Gestione BR Override Rosso / Arancio </v>
       </c>
       <c r="D4" s="23"/>
@@ -10805,7 +10917,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="23" t="str">
-        <f>VLOOKUP(B5,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B5,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v xml:space="preserve">trascinamento dello spegnimento segnale BR12 </v>
       </c>
       <c r="D5" s="23"/>
@@ -10859,7 +10971,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="23" t="str">
-        <f>VLOOKUP(B6,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B6,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>override NOPG</v>
       </c>
       <c r="D6" s="23"/>
@@ -10917,7 +11029,7 @@
         <v>78</v>
       </c>
       <c r="C7" s="23" t="str">
-        <f>VLOOKUP(B7,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B7,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>override ind.36</v>
       </c>
       <c r="D7" s="23"/>
@@ -10975,7 +11087,7 @@
         <v>95</v>
       </c>
       <c r="C8" s="23" t="str">
-        <f>VLOOKUP(B8,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B8,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>override Fitch Rosso</v>
       </c>
       <c r="D8" s="23"/>
@@ -11033,7 +11145,7 @@
         <v>104</v>
       </c>
       <c r="C9" s="23" t="str">
-        <f>VLOOKUP(B9,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B9,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>override Fitch Blu chiaro</v>
       </c>
       <c r="D9" s="23"/>
@@ -11089,7 +11201,7 @@
         <v>117</v>
       </c>
       <c r="C10" s="23" t="str">
-        <f>VLOOKUP(B10,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B10,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>override NOPG colore blu chiaro</v>
       </c>
       <c r="D10" s="23"/>
@@ -11147,7 +11259,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="23" t="str">
-        <f>VLOOKUP(B11,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B11,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>CR Esperienziali - nuovo indicatore e BR</v>
       </c>
       <c r="D11" s="23"/>
@@ -11203,7 +11315,7 @@
         <v>118</v>
       </c>
       <c r="C12" s="23" t="str">
-        <f>VLOOKUP(B12,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
+        <f>VLOOKUP(B12,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
         <v>intervento correttivo XRA</v>
       </c>
       <c r="D12" s="23"/>
@@ -11258,18 +11370,18 @@
     </row>
     <row r="13" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B13" s="22">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C13" s="23" t="str">
-        <f>VLOOKUP(B13,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>testare AQR per Banca BIB</v>
+        <f>VLOOKUP(B13,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Override - incrocio assegni (BR34)</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="23"/>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
@@ -11284,9 +11396,15 @@
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
+      <c r="X13" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y13" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="Z13" s="35" t="s">
+        <v>196</v>
+      </c>
       <c r="AA13" s="23"/>
       <c r="AB13" s="23"/>
       <c r="AC13" s="23"/>
@@ -11312,34 +11430,30 @@
     </row>
     <row r="14" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B14" s="22">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="23" t="str">
-        <f>VLOOKUP(B14,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>motore ALEX BANK</v>
+        <f>VLOOKUP(B14,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>testare AQR per Banca BIB</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
       <c r="R14" s="23"/>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
-      <c r="U14" s="29" t="s">
-        <v>196</v>
-      </c>
+      <c r="U14" s="23"/>
       <c r="V14" s="23"/>
       <c r="W14" s="23"/>
       <c r="X14" s="23"/>
@@ -11370,11 +11484,11 @@
     </row>
     <row r="15" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B15" s="22">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="23" t="str">
-        <f>VLOOKUP(B15,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>file test e TCK ALEX BANK</v>
+        <f>VLOOKUP(B15,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>motore ALEX BANK</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -11382,18 +11496,22 @@
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
       <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
+      <c r="O15" s="29" t="s">
+        <v>243</v>
+      </c>
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
       <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
+      <c r="U15" s="29" t="s">
+        <v>196</v>
+      </c>
       <c r="V15" s="23"/>
       <c r="W15" s="23"/>
       <c r="X15" s="23"/>
@@ -11424,47 +11542,35 @@
     </row>
     <row r="16" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B16" s="22">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" s="23" t="str">
-        <f>VLOOKUP(B16,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>motore CIB BANK</v>
+        <f>VLOOKUP(B16,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>file test e TCK ALEX BANK</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="28"/>
+      <c r="H16" s="23"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
-      <c r="M16" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
       <c r="V16" s="23"/>
-      <c r="W16" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="X16" s="28" t="s">
-        <v>198</v>
-      </c>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
       <c r="Y16" s="23"/>
-      <c r="Z16" s="28" t="s">
-        <v>196</v>
-      </c>
+      <c r="Z16" s="23"/>
       <c r="AA16" s="23"/>
       <c r="AB16" s="23"/>
       <c r="AC16" s="23"/>
@@ -11490,35 +11596,47 @@
     </row>
     <row r="17" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B17" s="22">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="23" t="str">
-        <f>VLOOKUP(B17,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>file test e TCK CIB BANK</v>
+        <f>VLOOKUP(B17,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>motore CIB BANK</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="M17" s="28" t="s">
+        <v>190</v>
+      </c>
       <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
+      <c r="O17" s="28"/>
       <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
+      <c r="Q17" s="28" t="s">
+        <v>198</v>
+      </c>
       <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
+      <c r="S17" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
       <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
+      <c r="W17" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="X17" s="28" t="s">
+        <v>198</v>
+      </c>
       <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="28" t="s">
+        <v>196</v>
+      </c>
       <c r="AA17" s="23"/>
       <c r="AB17" s="23"/>
       <c r="AC17" s="23"/>
@@ -11544,11 +11662,11 @@
     </row>
     <row r="18" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B18" s="22">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C18" s="23" t="str">
-        <f>VLOOKUP(B18,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>ISPRO - motore</v>
+        <f>VLOOKUP(B18,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>file test e TCK CIB BANK</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -11562,30 +11680,22 @@
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="R18" s="23"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
       <c r="Z18" s="23"/>
       <c r="AA18" s="23"/>
-      <c r="AB18" s="37" t="s">
-        <v>106</v>
-      </c>
+      <c r="AB18" s="23"/>
       <c r="AC18" s="23"/>
       <c r="AD18" s="23"/>
-      <c r="AE18" s="37" t="s">
-        <v>196</v>
-      </c>
+      <c r="AE18" s="23"/>
       <c r="AF18" s="23"/>
       <c r="AG18" s="23"/>
       <c r="AH18" s="23"/>
@@ -11606,11 +11716,11 @@
     </row>
     <row r="19" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B19" s="22">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="23" t="str">
-        <f>VLOOKUP(B19,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>ISPRO - file test e TCK</v>
+        <f>VLOOKUP(B19,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>ISPRO - motore</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -11625,21 +11735,29 @@
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
       <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
+      <c r="Q19" s="37" t="s">
+        <v>190</v>
+      </c>
       <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="S19" s="37"/>
       <c r="T19" s="37"/>
       <c r="U19" s="37"/>
       <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
+      <c r="W19" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
       <c r="Z19" s="23"/>
       <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
+      <c r="AB19" s="37" t="s">
+        <v>106</v>
+      </c>
       <c r="AC19" s="23"/>
       <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
+      <c r="AE19" s="37" t="s">
+        <v>196</v>
+      </c>
       <c r="AF19" s="23"/>
       <c r="AG19" s="23"/>
       <c r="AH19" s="23"/>
@@ -11660,11 +11778,11 @@
     </row>
     <row r="20" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B20" s="22">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C20" s="23" t="str">
-        <f>VLOOKUP(B20,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>Retail: costruzione file excel interno e verifica presenza Corporate</v>
+        <f>VLOOKUP(B20,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>ISPRO - file test e TCK</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -11674,7 +11792,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
-      <c r="L20" s="35"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
@@ -11682,76 +11800,43 @@
       <c r="Q20" s="23"/>
       <c r="R20" s="23"/>
       <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="37"/>
       <c r="X20" s="23"/>
       <c r="Y20" s="23"/>
       <c r="Z20" s="23"/>
-      <c r="AA20" s="35" t="s">
-        <v>242</v>
-      </c>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
       <c r="AC20" s="23"/>
       <c r="AD20" s="23"/>
-      <c r="AE20" s="35" t="s">
-        <v>106</v>
-      </c>
+      <c r="AE20" s="23"/>
       <c r="AF20" s="23"/>
       <c r="AG20" s="23"/>
-      <c r="AH20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AI20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AJ20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AK20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AL20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AO20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AP20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AQ20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AR20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AT20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AU20" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="AV20" s="35" t="s">
-        <v>196</v>
-      </c>
+      <c r="AH20" s="23"/>
+      <c r="AI20" s="23"/>
+      <c r="AJ20" s="23"/>
+      <c r="AK20" s="23"/>
+      <c r="AL20" s="23"/>
+      <c r="AM20" s="23"/>
+      <c r="AN20" s="23"/>
+      <c r="AO20" s="23"/>
+      <c r="AP20" s="23"/>
+      <c r="AQ20" s="23"/>
+      <c r="AR20" s="23"/>
+      <c r="AS20" s="23"/>
+      <c r="AT20" s="23"/>
+      <c r="AU20" s="23"/>
+      <c r="AV20" s="23"/>
     </row>
     <row r="21" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B21" s="22">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="23" t="str">
-        <f>VLOOKUP(B21,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>Retail: test di performance (2 mio di dati)</v>
+        <f>VLOOKUP(B21,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Retail: costruzione file excel interno e verifica presenza Corporate</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -11762,7 +11847,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
       <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
+      <c r="M21" s="23"/>
       <c r="N21" s="23"/>
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
@@ -11776,36 +11861,69 @@
       <c r="X21" s="23"/>
       <c r="Y21" s="23"/>
       <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
+      <c r="AA21" s="35" t="s">
+        <v>242</v>
+      </c>
       <c r="AC21" s="23"/>
       <c r="AD21" s="23"/>
-      <c r="AE21" s="23"/>
+      <c r="AE21" s="35" t="s">
+        <v>106</v>
+      </c>
       <c r="AF21" s="23"/>
       <c r="AG21" s="23"/>
-      <c r="AH21" s="23"/>
-      <c r="AI21" s="23"/>
-      <c r="AJ21" s="23"/>
-      <c r="AK21" s="23"/>
-      <c r="AL21" s="23"/>
-      <c r="AM21" s="23"/>
-      <c r="AN21" s="23"/>
-      <c r="AO21" s="23"/>
-      <c r="AP21" s="23"/>
-      <c r="AQ21" s="23"/>
-      <c r="AR21" s="23"/>
-      <c r="AS21" s="23"/>
-      <c r="AT21" s="23"/>
-      <c r="AU21" s="23"/>
-      <c r="AV21" s="23"/>
+      <c r="AH21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AM21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AP21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AQ21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU21" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV21" s="35" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="22" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B22" s="22">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C22" s="23" t="str">
-        <f>VLOOKUP(B22,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>VM - Retail: nodo Riempimento</v>
+        <f>VLOOKUP(B22,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Retail: test di performance (2 mio di dati)</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -11815,11 +11933,11 @@
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
       <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="23"/>
-      <c r="O22" s="119"/>
-      <c r="P22" s="119"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="23"/>
       <c r="R22" s="23"/>
       <c r="S22" s="23"/>
@@ -11853,13 +11971,13 @@
       <c r="AU22" s="23"/>
       <c r="AV22" s="23"/>
     </row>
-    <row r="23" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B23" s="22">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="23" t="str">
-        <f>VLOOKUP(B23,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>Retail: sviluppo indicatori</v>
+        <f>VLOOKUP(B23,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>VM - Retail: nodo Riempimento</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -11872,68 +11990,48 @@
       <c r="L23" s="23"/>
       <c r="M23" s="23"/>
       <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="R23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="S23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="T23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="U23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="V23" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="W23" s="119" t="s">
-        <v>189</v>
-      </c>
+      <c r="O23" s="119"/>
+      <c r="P23" s="119"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
       <c r="X23" s="23"/>
       <c r="Y23" s="23"/>
       <c r="Z23" s="23"/>
-      <c r="AA23" s="119" t="s">
-        <v>106</v>
-      </c>
+      <c r="AA23" s="23"/>
       <c r="AB23" s="23"/>
       <c r="AC23" s="23"/>
       <c r="AD23" s="23"/>
       <c r="AE23" s="23"/>
       <c r="AF23" s="23"/>
       <c r="AG23" s="23"/>
-      <c r="AH23" s="119" t="s">
-        <v>196</v>
-      </c>
-      <c r="AI23" s="1"/>
-      <c r="AJ23" s="1"/>
-      <c r="AK23" s="1"/>
-      <c r="AL23" s="1"/>
-      <c r="AM23" s="1"/>
-      <c r="AN23" s="1"/>
-      <c r="AO23" s="1"/>
-      <c r="AP23" s="1"/>
-      <c r="AQ23" s="1"/>
-      <c r="AR23" s="1"/>
-      <c r="AS23" s="1"/>
-      <c r="AT23" s="1"/>
-      <c r="AU23" s="1"/>
-      <c r="AV23" s="1"/>
+      <c r="AH23" s="23"/>
+      <c r="AI23" s="23"/>
+      <c r="AJ23" s="23"/>
+      <c r="AK23" s="23"/>
+      <c r="AL23" s="23"/>
+      <c r="AM23" s="23"/>
+      <c r="AN23" s="23"/>
+      <c r="AO23" s="23"/>
+      <c r="AP23" s="23"/>
+      <c r="AQ23" s="23"/>
+      <c r="AR23" s="23"/>
+      <c r="AS23" s="23"/>
+      <c r="AT23" s="23"/>
+      <c r="AU23" s="23"/>
+      <c r="AV23" s="23"/>
     </row>
     <row r="24" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="22">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="23" t="str">
-        <f>VLOOKUP(B24,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>Retail: configurazione start-up app (excel)</v>
+        <f>VLOOKUP(B24,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Retail: sviluppo indicatori</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -11947,22 +12045,38 @@
       <c r="M24" s="23"/>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="119"/>
-      <c r="U24" s="119"/>
-      <c r="V24" s="119"/>
-      <c r="W24" s="119"/>
-      <c r="X24" s="119"/>
-      <c r="Y24" s="119"/>
+      <c r="P24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="R24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="S24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="T24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="U24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="V24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="W24" s="119" t="s">
+        <v>189</v>
+      </c>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
       <c r="Z24" s="23"/>
-      <c r="AA24" s="23"/>
+      <c r="AA24" s="119" t="s">
+        <v>106</v>
+      </c>
       <c r="AB24" s="23"/>
-      <c r="AC24" s="119" t="s">
-        <v>106</v>
-      </c>
+      <c r="AC24" s="23"/>
       <c r="AD24" s="23"/>
       <c r="AE24" s="23"/>
       <c r="AF24" s="23"/>
@@ -11987,11 +12101,11 @@
     </row>
     <row r="25" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="22">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="23" t="str">
-        <f>VLOOKUP(B25,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>Retail: configurazione iniziale app e VM  (BR, Matrice e FT)</v>
+        <f>VLOOKUP(B25,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Retail: configurazione start-up app (excel)</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -12009,20 +12123,20 @@
       <c r="Q25" s="23"/>
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
+      <c r="T25" s="119"/>
       <c r="U25" s="119"/>
       <c r="V25" s="119"/>
       <c r="W25" s="119"/>
       <c r="X25" s="119"/>
       <c r="Y25" s="119"/>
-      <c r="Z25" s="119"/>
+      <c r="Z25" s="23"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
-      <c r="AC25" s="23"/>
+      <c r="AC25" s="119" t="s">
+        <v>106</v>
+      </c>
       <c r="AD25" s="23"/>
-      <c r="AE25" s="119" t="s">
-        <v>106</v>
-      </c>
+      <c r="AE25" s="23"/>
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
       <c r="AH25" s="119" t="s">
@@ -12045,11 +12159,11 @@
     </row>
     <row r="26" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="22">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C26" s="23" t="str">
-        <f>VLOOKUP(B26,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>ISBA - motore</v>
+        <f>VLOOKUP(B26,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>Retail: configurazione iniziale app e VM  (BR, Matrice e FT)</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -12068,26 +12182,22 @@
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="W26" s="23"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="AB26" s="38"/>
-      <c r="AC26" s="38"/>
-      <c r="AD26" s="38"/>
-      <c r="AE26" s="38" t="s">
+      <c r="U26" s="119"/>
+      <c r="V26" s="119"/>
+      <c r="W26" s="119"/>
+      <c r="X26" s="119"/>
+      <c r="Y26" s="119"/>
+      <c r="Z26" s="119"/>
+      <c r="AA26" s="23"/>
+      <c r="AB26" s="23"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="23"/>
+      <c r="AE26" s="119" t="s">
         <v>106</v>
       </c>
       <c r="AF26" s="23"/>
       <c r="AG26" s="23"/>
-      <c r="AH26" s="38" t="s">
+      <c r="AH26" s="119" t="s">
         <v>196</v>
       </c>
       <c r="AI26" s="1"/>
@@ -12105,13 +12215,13 @@
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
     </row>
-    <row r="27" spans="2:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="22">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="23" t="str">
-        <f>VLOOKUP(B27,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>ISBA - file test e TCK</v>
+        <f>VLOOKUP(B27,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>ISBA - motore</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -12131,41 +12241,49 @@
       <c r="S27" s="23"/>
       <c r="T27" s="23"/>
       <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
+      <c r="V27" s="38" t="s">
+        <v>190</v>
+      </c>
       <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
-      <c r="Y27" s="23"/>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="AB27" s="38"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="23"/>
-      <c r="AE27" s="23"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="38" t="s">
+        <v>106</v>
+      </c>
       <c r="AF27" s="23"/>
       <c r="AG27" s="23"/>
-      <c r="AH27" s="23"/>
-      <c r="AI27" s="23"/>
-      <c r="AJ27" s="23"/>
-      <c r="AK27" s="23"/>
-      <c r="AL27" s="23"/>
-      <c r="AM27" s="23"/>
-      <c r="AN27" s="23"/>
-      <c r="AO27" s="23"/>
-      <c r="AP27" s="23"/>
-      <c r="AQ27" s="23"/>
-      <c r="AR27" s="23"/>
-      <c r="AS27" s="23"/>
-      <c r="AT27" s="23"/>
-      <c r="AU27" s="23"/>
-      <c r="AV27" s="23"/>
-    </row>
-    <row r="28" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH27" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+    </row>
+    <row r="28" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B28" s="22">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C28" s="23" t="str">
-        <f>VLOOKUP(B28,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>APP2.0 - Configurazione</v>
+        <f>VLOOKUP(B28,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>ISBA - file test e TCK</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -12184,42 +12302,42 @@
       <c r="R28" s="23"/>
       <c r="S28" s="23"/>
       <c r="T28" s="23"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="121"/>
-      <c r="W28" s="121"/>
-      <c r="X28" s="121"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="121"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="121"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="121"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
-      <c r="AL28" s="1"/>
-      <c r="AM28" s="1"/>
-      <c r="AN28" s="1"/>
-      <c r="AO28" s="1"/>
-      <c r="AP28" s="1"/>
-      <c r="AQ28" s="1"/>
-      <c r="AR28" s="1"/>
-      <c r="AS28" s="1"/>
-      <c r="AT28" s="1"/>
-      <c r="AU28" s="1"/>
-      <c r="AV28" s="1"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="38"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="23"/>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="23"/>
+      <c r="AJ28" s="23"/>
+      <c r="AK28" s="23"/>
+      <c r="AL28" s="23"/>
+      <c r="AM28" s="23"/>
+      <c r="AN28" s="23"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="23"/>
+      <c r="AQ28" s="23"/>
+      <c r="AR28" s="23"/>
+      <c r="AS28" s="23"/>
+      <c r="AT28" s="23"/>
+      <c r="AU28" s="23"/>
+      <c r="AV28" s="23"/>
     </row>
     <row r="29" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="22">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="23" t="str">
-        <f>VLOOKUP(B29,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>APP2.0 - Migrazione</v>
+        <f>VLOOKUP(B29,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>APP2.0 - Configurazione</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -12242,13 +12360,13 @@
       <c r="V29" s="121"/>
       <c r="W29" s="121"/>
       <c r="X29" s="121"/>
-      <c r="Y29" s="121"/>
+      <c r="Y29" s="1"/>
       <c r="Z29" s="121"/>
-      <c r="AA29" s="121"/>
+      <c r="AA29" s="1"/>
       <c r="AB29" s="121"/>
-      <c r="AC29" s="121"/>
+      <c r="AC29" s="1"/>
       <c r="AD29" s="121"/>
-      <c r="AE29" s="121"/>
+      <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
@@ -12267,13 +12385,13 @@
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
     </row>
-    <row r="30" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:48" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="22">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="23" t="str">
-        <f>VLOOKUP(B30,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v xml:space="preserve">SME Retail - fil excel </v>
+        <f>VLOOKUP(B30,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>APP2.0 - Migrazione</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -12293,16 +12411,16 @@
       <c r="S30" s="23"/>
       <c r="T30" s="23"/>
       <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
+      <c r="V30" s="121"/>
+      <c r="W30" s="121"/>
+      <c r="X30" s="121"/>
+      <c r="Y30" s="121"/>
+      <c r="Z30" s="121"/>
+      <c r="AA30" s="121"/>
+      <c r="AB30" s="121"/>
+      <c r="AC30" s="121"/>
+      <c r="AD30" s="121"/>
+      <c r="AE30" s="121"/>
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
@@ -12323,11 +12441,11 @@
     </row>
     <row r="31" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="22">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="23" t="str">
-        <f>VLOOKUP(B31,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>SME Retail - AFU</v>
+        <f>VLOOKUP(B31,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v xml:space="preserve">SME Retail - fil excel </v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -12346,18 +12464,14 @@
       <c r="R31" s="23"/>
       <c r="S31" s="23"/>
       <c r="T31" s="23"/>
-      <c r="U31" s="117" t="s">
-        <v>456</v>
-      </c>
+      <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
-      <c r="AB31" s="117" t="s">
-        <v>190</v>
-      </c>
+      <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
@@ -12381,11 +12495,11 @@
     </row>
     <row r="32" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="22">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="23" t="str">
-        <f>VLOOKUP(B32,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>SME Retail - Sviluppo indicatori</v>
+        <f>VLOOKUP(B32,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>SME Retail - AFU</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -12404,41 +12518,27 @@
       <c r="R32" s="23"/>
       <c r="S32" s="23"/>
       <c r="T32" s="23"/>
-      <c r="U32" s="1"/>
+      <c r="U32" s="117" t="s">
+        <v>456</v>
+      </c>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
-      <c r="Z32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AF32" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="AG32" s="118" t="s">
-        <v>189</v>
-      </c>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="117" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
-      <c r="AK32" s="120" t="s">
-        <v>106</v>
-      </c>
+      <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
@@ -12453,11 +12553,11 @@
     </row>
     <row r="33" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="22">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="23" t="str">
-        <f>VLOOKUP(B33,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>SME Retail - test indicatori</v>
+        <f>VLOOKUP(B33,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>SME Retail - Sviluppo indicatori</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -12525,11 +12625,11 @@
     </row>
     <row r="34" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="22">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="23" t="str">
-        <f>VLOOKUP(B34,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>SME Retail - Configurazione start-up app (excel)</v>
+        <f>VLOOKUP(B34,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>SME Retail - test indicatori</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="23"/>
@@ -12553,18 +12653,36 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-      <c r="AE34" s="1"/>
-      <c r="AF34" s="120"/>
-      <c r="AG34" s="120"/>
-      <c r="AH34" s="120"/>
-      <c r="AI34" s="120"/>
-      <c r="AJ34" s="120"/>
-      <c r="AK34" s="1"/>
+      <c r="Z34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AG34" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+      <c r="AK34" s="120" t="s">
+        <v>106</v>
+      </c>
       <c r="AL34" s="1"/>
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
@@ -12579,11 +12697,11 @@
     </row>
     <row r="35" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="22">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="23" t="str">
-        <f>VLOOKUP(B35,Elenco_attività!$B$47:$C$313,2,FALSE)</f>
-        <v>SME Retail - Configurazione iniziale app e VM  (BR, Matrice e FT)</v>
+        <f>VLOOKUP(B35,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>SME Retail - Configurazione start-up app (excel)</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="23"/>
@@ -12631,116 +12749,170 @@
       <c r="AU35" s="1"/>
       <c r="AV35" s="1"/>
     </row>
-    <row r="36" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B38" s="35"/>
-      <c r="C38" s="16" t="s">
+    <row r="36" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="22">
+        <v>129</v>
+      </c>
+      <c r="C36" s="23" t="str">
+        <f>VLOOKUP(B36,Elenco_attività!$B$47:$C$314,2,FALSE)</f>
+        <v>SME Retail - Configurazione iniziale app e VM  (BR, Matrice e FT)</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="120"/>
+      <c r="AG36" s="120"/>
+      <c r="AH36" s="120"/>
+      <c r="AI36" s="120"/>
+      <c r="AJ36" s="120"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="1"/>
+      <c r="AQ36" s="1"/>
+      <c r="AR36" s="1"/>
+      <c r="AS36" s="1"/>
+      <c r="AT36" s="1"/>
+      <c r="AU36" s="1"/>
+      <c r="AV36" s="1"/>
+    </row>
+    <row r="37" spans="2:48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B39" s="35"/>
+      <c r="C39" s="16" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="39" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B39" s="24"/>
-      <c r="C39" s="16" t="s">
+    <row r="40" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B40" s="24"/>
+      <c r="C40" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B40" s="25"/>
-      <c r="C40" s="16" t="s">
+    <row r="41" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B41" s="25"/>
+      <c r="C41" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B41" s="119"/>
-      <c r="C41" s="16" t="s">
+    <row r="42" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B42" s="119"/>
+      <c r="C42" s="16" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="42" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B42" s="27"/>
-      <c r="C42" s="16" t="s">
+    <row r="43" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B43" s="27"/>
+      <c r="C43" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B43" s="36"/>
-      <c r="C43" s="16" t="s">
+    <row r="44" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B44" s="36"/>
+      <c r="C44" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B44" s="30"/>
-      <c r="C44" s="16" t="s">
+    <row r="45" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B45" s="30"/>
+      <c r="C45" s="16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B45" s="117"/>
-      <c r="C45" s="16" t="s">
+    <row r="46" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B46" s="117"/>
+      <c r="C46" s="16" t="s">
         <v>459</v>
-      </c>
-    </row>
-    <row r="47" spans="2:48" x14ac:dyDescent="0.3">
-      <c r="B47" s="60">
-        <v>42782</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="48" spans="2:48" x14ac:dyDescent="0.3">
       <c r="B48" s="60">
-        <v>42786</v>
+        <v>42782</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="60">
-        <v>42790</v>
+        <v>42786</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="60">
-        <v>42786</v>
+        <v>42790</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="60">
-        <v>42796</v>
+        <v>42786</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="60">
-        <v>42797</v>
+        <v>42796</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="60">
-        <v>42802</v>
+        <v>42797</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>249</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="60">
+        <v>42802</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="60">
         <v>42803</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C55" s="16" t="s">
         <v>250</v>
       </c>
     </row>
@@ -12759,7 +12931,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="AU12" sqref="AU12"/>
+      <selection pane="bottomRight" activeCell="BC12" sqref="BC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -12969,11 +13141,11 @@
       </c>
       <c r="AV1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="AW1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="AX1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -15769,10 +15941,10 @@
   <dimension ref="B1:FU16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG1" sqref="AG1"/>
+      <selection pane="bottomRight" activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -15928,11 +16100,11 @@
       </c>
       <c r="AK1" s="64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="AL1" s="64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="AM1" s="64" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -17894,7 +18066,9 @@
       <c r="AV7" s="73" t="s">
         <v>396</v>
       </c>
-      <c r="AW7" s="68"/>
+      <c r="AW7" s="69" t="s">
+        <v>259</v>
+      </c>
       <c r="AX7" s="68"/>
       <c r="AY7" s="68"/>
       <c r="AZ7" s="68"/>
@@ -18233,7 +18407,7 @@
       <c r="AV8" s="61"/>
       <c r="AW8" s="61">
         <f>COUNTBLANK(AW3:AW7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX8" s="61">
         <f>COUNTBLANK(AX3:AX7)</f>

</xml_diff>

<commit_message>
update HP da Corp
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
+++ b/earlywarning-pom/Document/SpecificheIndicatori/Attivita.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9216" windowHeight="5316" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9216" windowHeight="5316"/>
   </bookViews>
   <sheets>
     <sheet name="Elenco_attività" sheetId="1" r:id="rId1"/>
@@ -3982,8 +3982,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AE156"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6850,7 +6850,9 @@
       <c r="E99" s="13">
         <v>1</v>
       </c>
-      <c r="F99" s="13"/>
+      <c r="F99" s="13">
+        <v>1</v>
+      </c>
       <c r="G99" s="13"/>
       <c r="H99" s="5">
         <v>2</v>
@@ -7354,7 +7356,9 @@
       <c r="E117" s="13">
         <v>1</v>
       </c>
-      <c r="F117" s="13"/>
+      <c r="F117" s="13">
+        <v>1</v>
+      </c>
       <c r="G117" s="13"/>
       <c r="H117" s="5">
         <v>2</v>
@@ -7464,7 +7468,9 @@
       <c r="E121" s="13">
         <v>1</v>
       </c>
-      <c r="F121" s="13"/>
+      <c r="F121" s="13">
+        <v>1</v>
+      </c>
       <c r="G121" s="13"/>
       <c r="H121" s="5">
         <v>3</v>
@@ -7510,7 +7516,7 @@
         <v>398</v>
       </c>
       <c r="E123" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F123" s="13"/>
       <c r="G123" s="13"/>
@@ -7530,7 +7536,7 @@
         <v>398</v>
       </c>
       <c r="E124" s="13">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
@@ -7552,7 +7558,9 @@
       <c r="E125" s="13">
         <v>1</v>
       </c>
-      <c r="F125" s="13"/>
+      <c r="F125" s="13">
+        <v>1</v>
+      </c>
       <c r="G125" s="13"/>
       <c r="H125" s="5">
         <v>3</v>
@@ -7597,7 +7605,9 @@
       <c r="D127" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E127" s="13"/>
+      <c r="E127" s="13">
+        <v>0.25</v>
+      </c>
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
       <c r="H127" s="5">
@@ -7619,7 +7629,9 @@
       <c r="D128" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E128" s="13"/>
+      <c r="E128" s="13">
+        <v>0.25</v>
+      </c>
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="5">
@@ -7641,7 +7653,9 @@
       <c r="D129" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E129" s="13"/>
+      <c r="E129" s="13">
+        <v>0.25</v>
+      </c>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="5">
@@ -7711,7 +7725,9 @@
       <c r="D132" s="17" t="s">
         <v>467</v>
       </c>
-      <c r="E132" s="13"/>
+      <c r="E132" s="13">
+        <v>0.5</v>
+      </c>
       <c r="F132" s="13"/>
       <c r="G132" s="13"/>
       <c r="H132" s="5">
@@ -7786,8 +7802,12 @@
       <c r="E135" s="13">
         <v>1</v>
       </c>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
+      <c r="F135" s="13">
+        <v>1</v>
+      </c>
+      <c r="G135" s="13">
+        <v>1</v>
+      </c>
       <c r="H135" s="5">
         <v>2</v>
       </c>
@@ -10680,10 +10700,10 @@
   <dimension ref="B1:AV55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="Y21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Y24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB33" sqref="AB33"/>
+      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -10826,11 +10846,11 @@
       </c>
       <c r="AF1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="AG1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="AH1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -13159,11 +13179,11 @@
   <dimension ref="B1:DR23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="CL2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="CE12" sqref="CE12"/>
+      <selection pane="bottomRight" activeCell="CZ15" sqref="CZ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -13589,7 +13609,7 @@
       </c>
       <c r="CX1" s="26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="CY1" s="26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -13597,7 +13617,7 @@
       </c>
       <c r="CZ1" s="26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="DA1" s="26" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -16172,11 +16192,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="CP3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="CJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CP4" sqref="CP4"/>
+      <selection pane="bottomRight" activeCell="DD1" sqref="DD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -16551,7 +16571,7 @@
       </c>
       <c r="CM1" s="64" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="CN1" s="64" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -16559,7 +16579,7 @@
       </c>
       <c r="CO1" s="64" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="CP1" s="64" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>